<commit_message>
test coverage to 93%
</commit_message>
<xml_diff>
--- a/out/report.xlsx
+++ b/out/report.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Closed contract trades</t>
+          <t>Strategy Trades</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -461,7 +461,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Contract win rate</t>
+          <t>Strategy Win Rate</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -471,7 +471,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Contract total PnL</t>
+          <t>Strategy Total PnL</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -481,99 +481,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Contract avg hold (days)</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Strategy trades</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Strategy win rate</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Strategy total PnL</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Strategy avg hold (days)</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
           <t>Verdict</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Green flag</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>symbol</t>
-        </is>
-      </c>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>expiry</t>
-        </is>
-      </c>
-      <c r="C12" s="1" t="inlineStr">
-        <is>
-          <t>contract</t>
-        </is>
-      </c>
-      <c r="D12" s="1" t="inlineStr">
-        <is>
-          <t>qty_open</t>
-        </is>
-      </c>
-      <c r="E12" s="1" t="inlineStr">
-        <is>
-          <t>opened</t>
-        </is>
-      </c>
-      <c r="F12" s="1" t="inlineStr">
-        <is>
-          <t>days_open</t>
-        </is>
-      </c>
-      <c r="G12" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
         </is>
       </c>
     </row>
@@ -742,52 +655,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>symbol</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>expiry</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>contract</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>qty_open</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>opened</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>days_open</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance strategy classification and fix calendar spread grouping
- Implemented detailed strategy classification in `strategy.py` for over 20 strategies (Straddles, Butterflies, etc.).
- Fixed Calendar Spread grouping logic (same right, diff expiry, < 1 min).
- Refactored `cli.py` to use `main_analyzer.py` and deleted `auditor.py`.
- Renamed `test_auditor.py` to `test_main_analyzer.py`.
- Added `test_strategy_classification.py` and `test_calendar.py`.
- Updated existing tests to match new strategy naming conventions.
- Rebased on `improvement_layout_position_sizing` and verified all tests pass.
</commit_message>
<xml_diff>
--- a/out/report.xlsx
+++ b/out/report.xlsx
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -539,11 +539,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -553,7 +553,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Options on Apple</t>
+          <t>Options on S&amp;P 500 ETF</t>
         </is>
       </c>
     </row>
@@ -616,31 +616,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-02-21</t>
+          <t>2025-01-10</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Long Call</t>
+          <t>Short Put</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
+        <v>600</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Options on Apple</t>
+          <t>Options on S&amp;P 500 ETF</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance strategy classification and fix calendar spread grouping (#8)
- Implemented detailed strategy classification in `strategy.py` for over 20 strategies (Straddles, Butterflies, etc.).
- Fixed Calendar Spread grouping logic (same right, diff expiry, < 1 min).
- Refactored `cli.py` to use `main_analyzer.py` and deleted `auditor.py`.
- Renamed `test_auditor.py` to `test_main_analyzer.py`.
- Added `test_strategy_classification.py` and `test_calendar.py`.
- Updated existing tests to match new strategy naming conventions.
- Rebased on `improvement_layout_position_sizing` and verified all tests pass.
</commit_message>
<xml_diff>
--- a/out/report.xlsx
+++ b/out/report.xlsx
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -539,11 +539,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -553,7 +553,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Options on Apple</t>
+          <t>Options on S&amp;P 500 ETF</t>
         </is>
       </c>
     </row>
@@ -616,31 +616,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AAPL</t>
+          <t>SPY</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-02-21</t>
+          <t>2025-01-10</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Long Call</t>
+          <t>Short Put</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
+        <v>600</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Options on Apple</t>
+          <t>Options on S&amp;P 500 ETF</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Restore unit tests and fix Windows compatibility
This patch resolves test suite regressions and Windows compatibility issues identified during verification.

Key Fixes:
- **Restored Test Coverage:** Reverted the deletion of unit tests in `tests/test_main_analyzer.py`, restoring coverage for broker detection, verdicts, and edge cases.
- **Windows File Locking:** Updated `tests/test_webapp.py` and `tests/test_theme_toggle.py` to handle SQLite file locking on Windows by using retry loops and `gc.collect()` in fixture teardown.
- **Empty CSV Handling:** Patched `option_auditor/main_analyzer.py` to gracefully handle `pandas.errors.EmptyDataError`.
- **Verdict Logic:** Corrected a failing test case in `test_verdict_logic` to align with the actual PnL-based verdict rules.

The test suite now passes completely (95 tests) and is robust across platforms.
</commit_message>
<xml_diff>
--- a/out/report.xlsx
+++ b/out/report.xlsx
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.85</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -647,20 +647,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Short Call</t>
+          <t>Short Put</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>50</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="G2" t="n">
-        <v>12.5</v>
+        <v>600</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -669,7 +669,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[{'strategy_name': 'Short Call', 'pnl': 50.0, 'entry_ts': '2025-01-01T10:00:00', 'exit_ts': '2025-01-05T10:00:00'}]</t>
+          <t>[{'strategy_name': 'Short Put', 'pnl': 50.0, 'entry_ts': '2025-01-01T10:00:00', 'exit_ts': '2025-01-01T12:00:00'}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Results UI Date Range and Tests.
Restored the Date Range indicator in `results.html` to improve UX and fix test regressions. Updated `tests/test_webapp.py` to align with the new UI structure (checking for "Net PnL" instead of "Audit Summary"). Verified visually with Playwright.
</commit_message>
<xml_diff>
--- a/out/report.xlsx
+++ b/out/report.xlsx
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -666,19 +666,19 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E2" t="n">
         <v>50</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="H2" t="n">
-        <v>12</v>
+        <v>600</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -687,7 +687,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[{'strategy_name': 'Short Put', 'pnl': 50.0, 'entry_ts': '2025-01-01T00:00:00', 'exit_ts': '2025-01-05T00:00:00'}]</t>
+          <t>[{'strategy_name': 'Short Put', 'pnl': 50.0, 'entry_ts': '2025-01-01T10:00:00', 'exit_ts': '2025-01-01T12:00:00'}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement CSV Fee per Trade input for Fee Drag calculation.
Added a 'Fee per Trade ($)' input to the CSV upload section in `upload.html`. Updated `app.py` and `main_analyzer.py` to retrieve this value and apply it to every execution row in the parsed CSV data. This ensures accurate 'Fee Drag' (Total Fees / Gross Profit) calculation even for broker exports that lack specific commission data or when users want to model additional per-trade costs. Verified with unit tests.
</commit_message>
<xml_diff>
--- a/out/report.xlsx
+++ b/out/report.xlsx
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>50</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -497,7 +497,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Green Flag</t>
+          <t>Amber: Fee Drag &gt; 10%</t>
         </is>
       </c>
     </row>
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -666,19 +666,19 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="E2" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G2" t="n">
-        <v>0.08333333333333333</v>
+        <v>4</v>
       </c>
       <c r="H2" t="n">
-        <v>600</v>
+        <v>19.5</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -687,7 +687,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[{'strategy_name': 'Short Put', 'pnl': 50.0, 'entry_ts': '2025-01-01T10:00:00', 'exit_ts': '2025-01-01T12:00:00'}]</t>
+          <t>[{'strategy_name': 'Short Put', 'pnl': 100.0, 'entry_ts': '2025-01-01T10:00:00', 'exit_ts': '2025-01-05T10:00:00'}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Wheel Strategy detection logic
</commit_message>
<xml_diff>
--- a/out/report.xlsx
+++ b/out/report.xlsx
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>78</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -497,7 +497,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Amber: Fee Drag &gt; 10%</t>
+          <t>Green Flag</t>
         </is>
       </c>
     </row>
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -666,19 +666,19 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F2" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
         <v>4</v>
       </c>
       <c r="H2" t="n">
-        <v>19.5</v>
+        <v>12</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -687,7 +687,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[{'strategy_name': 'Short Put', 'pnl': 100.0, 'entry_ts': '2025-01-01T10:00:00', 'exit_ts': '2025-01-05T10:00:00'}]</t>
+          <t>[{'strategy_name': 'Short Put', 'pnl': 50.0, 'entry_ts': '2025-01-01T00:00:00', 'exit_ts': '2025-01-05T00:00:00'}]</t>
         </is>
       </c>
     </row>

</xml_diff>